<commit_message>
updates Lions team evidence file
</commit_message>
<xml_diff>
--- a/mcanvar/evidence.xlsx
+++ b/mcanvar/evidence.xlsx
@@ -8,43 +8,43 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mevlutcanvar/repos/temp/gon-evidence/mcanvar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DBEC9E-D096-7D4D-852C-9C426FE9B718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66DE60F-8242-A742-8C04-6BF8BA268E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="32540" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="500" windowWidth="16260" windowHeight="20500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Info - Tablo 1" sheetId="1" r:id="rId1"/>
-    <sheet name="A1 - Tablo 1" sheetId="2" r:id="rId2"/>
-    <sheet name="A2 - Tablo 1" sheetId="3" r:id="rId3"/>
-    <sheet name="A3 - Tablo 1" sheetId="4" r:id="rId4"/>
-    <sheet name="A4 - Tablo 1" sheetId="5" r:id="rId5"/>
-    <sheet name="A5 - Tablo 1" sheetId="6" r:id="rId6"/>
-    <sheet name="A6 - Tablo 1" sheetId="7" r:id="rId7"/>
-    <sheet name="A7 - Tablo 1" sheetId="8" r:id="rId8"/>
-    <sheet name="A8 - Tablo 1" sheetId="9" r:id="rId9"/>
-    <sheet name="A9 - Tablo 1" sheetId="10" r:id="rId10"/>
-    <sheet name="A10 - Tablo 1" sheetId="11" r:id="rId11"/>
-    <sheet name="A11 - Tablo 1" sheetId="12" r:id="rId12"/>
-    <sheet name="A12 - Tablo 1" sheetId="13" r:id="rId13"/>
-    <sheet name="A13 - Tablo 1" sheetId="14" r:id="rId14"/>
-    <sheet name="A14 - Tablo 1" sheetId="15" r:id="rId15"/>
-    <sheet name="A15 - Tablo 1" sheetId="16" r:id="rId16"/>
-    <sheet name="A16 - Tablo 1" sheetId="17" r:id="rId17"/>
-    <sheet name="A17 - Tablo 1" sheetId="18" r:id="rId18"/>
-    <sheet name="A18 - Tablo 1" sheetId="19" r:id="rId19"/>
-    <sheet name="A19 - Tablo 1" sheetId="20" r:id="rId20"/>
-    <sheet name="A20 - Tablo 1" sheetId="21" r:id="rId21"/>
-    <sheet name="B1 - Tablo 1" sheetId="22" r:id="rId22"/>
-    <sheet name="B2 - Tablo 1" sheetId="23" r:id="rId23"/>
-    <sheet name="B5 - Tablo 1" sheetId="24" r:id="rId24"/>
-    <sheet name="B6 - Tablo 1" sheetId="25" r:id="rId25"/>
+    <sheet name="Info" sheetId="1" r:id="rId1"/>
+    <sheet name="A1" sheetId="2" r:id="rId2"/>
+    <sheet name="A2" sheetId="3" r:id="rId3"/>
+    <sheet name="A3" sheetId="4" r:id="rId4"/>
+    <sheet name="A4" sheetId="5" r:id="rId5"/>
+    <sheet name="A5" sheetId="6" r:id="rId6"/>
+    <sheet name="A6" sheetId="7" r:id="rId7"/>
+    <sheet name="A7" sheetId="8" r:id="rId8"/>
+    <sheet name="A8" sheetId="9" r:id="rId9"/>
+    <sheet name="A9" sheetId="10" r:id="rId10"/>
+    <sheet name="A10" sheetId="11" r:id="rId11"/>
+    <sheet name="A11" sheetId="12" r:id="rId12"/>
+    <sheet name="A12" sheetId="13" r:id="rId13"/>
+    <sheet name="A13" sheetId="14" r:id="rId14"/>
+    <sheet name="A14" sheetId="15" r:id="rId15"/>
+    <sheet name="A15" sheetId="16" r:id="rId16"/>
+    <sheet name="A16" sheetId="17" r:id="rId17"/>
+    <sheet name="A17" sheetId="18" r:id="rId18"/>
+    <sheet name="A18" sheetId="19" r:id="rId19"/>
+    <sheet name="A19" sheetId="20" r:id="rId20"/>
+    <sheet name="A20" sheetId="21" r:id="rId21"/>
+    <sheet name="B1" sheetId="22" r:id="rId22"/>
+    <sheet name="B2" sheetId="23" r:id="rId23"/>
+    <sheet name="B5" sheetId="24" r:id="rId24"/>
+    <sheet name="B6" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="50">
   <si>
     <t>TeamName</t>
   </si>
@@ -109,27 +109,15 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
     <t>nft id</t>
   </si>
   <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
     <t>ibc class on chain</t>
   </si>
   <si>
@@ -211,10 +199,10 @@
     <t>112E469943B5A7435173F39E0DA55D01C0B53F5AFCA94024BD48910D87623C22</t>
   </si>
   <si>
-    <t>gon-irishub-1</t>
-  </si>
-  <si>
     <t>F33A0343CB20FB1D2F07FADBB66FB2FC39956703D903DA419AF8DB48B9577B77</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -1534,7 +1522,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1692,7 +1680,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -1700,10 +1688,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1792,7 +1780,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -1800,10 +1788,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1892,7 +1880,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -1900,10 +1888,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1992,7 +1980,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2000,10 +1988,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2092,7 +2080,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2100,10 +2088,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2111,7 +2099,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2120,7 +2108,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2196,7 +2184,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2204,10 +2192,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2215,7 +2203,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2224,7 +2212,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2300,7 +2288,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2308,10 +2296,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2319,7 +2307,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2328,7 +2316,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2404,7 +2392,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2412,10 +2400,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2423,7 +2411,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2432,7 +2420,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2505,10 +2493,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2516,10 +2504,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2527,7 +2515,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2536,7 +2524,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2612,7 +2600,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2620,10 +2608,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2631,7 +2619,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2640,7 +2628,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2702,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2727,10 +2715,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2819,7 +2807,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2827,10 +2815,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2838,7 +2826,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2847,7 +2835,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2923,7 +2911,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -2931,10 +2919,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2942,7 +2930,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2951,7 +2939,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3032,7 +3020,7 @@
     </row>
     <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3041,7 +3029,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3130,7 +3118,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3139,7 +3127,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3228,7 +3216,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3237,7 +3225,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3307,7 +3295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3326,7 +3316,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3335,7 +3325,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3426,85 +3416,85 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -3537,7 +3527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3559,25 +3549,25 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5"/>
     </row>
@@ -3647,10 +3637,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3670,41 +3660,33 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>23</v>
+    <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>49</v>
-      </c>
+    <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3748,13 +3730,6 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -3767,10 +3742,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3790,41 +3765,33 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>23</v>
+    <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3868,13 +3835,6 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -3887,10 +3847,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3911,41 +3871,33 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>23</v>
+    <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3989,13 +3941,6 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -4024,7 +3969,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -4032,10 +3977,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -4124,7 +4069,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="5"/>
@@ -4132,10 +4077,10 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>

</xml_diff>